<commit_message>
changed swelling to each concentration. Other changes...
</commit_message>
<xml_diff>
--- a/tests/swellingpostprocessor/test.xlsx
+++ b/tests/swellingpostprocessor/test.xlsx
@@ -19,39 +19,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
-    <t>c1*r1</t>
+    <t>+----------------+----------------+----------------+----------------+----------------+----------------+----------------+----------------+</t>
   </si>
   <si>
-    <t>c2*r2</t>
+    <t>time</t>
   </si>
   <si>
-    <t>Sum</t>
+    <t>c1</t>
   </si>
   <si>
-    <t>+----------------+----------------+----------------+----------------+----------------+----------------+----------------+</t>
+    <t>c2</t>
   </si>
   <si>
-    <t xml:space="preserve"> time           </t>
+    <t>c3</t>
   </si>
   <si>
-    <t xml:space="preserve"> c1             </t>
+    <t>swelling_c1</t>
   </si>
   <si>
-    <t xml:space="preserve"> c2             </t>
+    <t>swelling_c2</t>
   </si>
   <si>
-    <t xml:space="preserve"> r1             </t>
+    <t>swelling_c3</t>
   </si>
   <si>
-    <t xml:space="preserve"> r2             </t>
+    <t>total_swelling</t>
   </si>
   <si>
-    <t xml:space="preserve"> swelling       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> total          </t>
+    <t>radius</t>
   </si>
 </sst>
 </file>
@@ -106,8 +103,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -131,7 +130,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -139,6 +138,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -146,6 +146,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -475,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P33"/>
+  <dimension ref="C2:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G5"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -490,188 +491,529 @@
     <col min="11" max="16" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" t="s">
+    <row r="2" spans="3:16">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2.7564659999999998E-4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3.4834770000000001E-4</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3.9960540000000001E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16">
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="3:16">
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="3:16">
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="B2" t="s">
+      <c r="G8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J8" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="K8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="B4" s="1">
-        <v>100</v>
-      </c>
-      <c r="C4" s="1">
-        <v>8352281000</v>
-      </c>
-      <c r="D4" s="1">
-        <v>823859400</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2.7564659999999998E-4</v>
-      </c>
-      <c r="F4" s="1">
-        <v>3.4834770000000001E-4</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.87861809999999996</v>
-      </c>
-      <c r="H4" s="1">
-        <v>10000000000</v>
-      </c>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="B5" s="1">
-        <v>200</v>
-      </c>
-      <c r="C5" s="1">
-        <v>7146103000</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1426948000</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2.7564659999999998E-4</v>
-      </c>
-      <c r="F5" s="1">
-        <v>3.4834770000000001E-4</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0.87958510000000001</v>
-      </c>
-      <c r="H5" s="1">
-        <v>10000000000</v>
-      </c>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="D8" t="s">
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+    </row>
+    <row r="9" spans="3:16">
+      <c r="C9" t="s">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="D9" s="1">
-        <f>C4*4/3*PI()*E4^3</f>
-        <v>0.73274291242834932</v>
-      </c>
-      <c r="E9" s="1">
-        <f>D4*4/3*PI()*F4^3</f>
-        <v>0.14587489376346446</v>
-      </c>
-      <c r="G9" s="5">
-        <f>SUM(D9:E9)</f>
-        <v>0.87861780619181373</v>
-      </c>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="H9" s="5"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+    </row>
+    <row r="10" spans="3:16">
       <c r="D10" s="1">
-        <f>C5*4/3*PI()*E5^3</f>
-        <v>0.62692530636037802</v>
+        <v>1000000</v>
       </c>
       <c r="E10" s="1">
-        <f>D5*4/3*PI()*F5^3</f>
-        <v>0.25265948037491359</v>
-      </c>
-      <c r="G10" s="5">
-        <f>SUM(D10:E10)</f>
-        <v>0.87958478673529161</v>
-      </c>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="L11" s="1"/>
-    </row>
-    <row r="17" spans="8:16">
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="8:16">
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="8:16">
-      <c r="H19" s="5"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-    </row>
-    <row r="20" spans="8:16">
-      <c r="H20" s="5"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-    </row>
-    <row r="21" spans="8:16">
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="8:16">
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="8:16">
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="8:16">
-      <c r="H24" s="5"/>
-    </row>
-    <row r="29" spans="8:16">
-      <c r="H29" s="2"/>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="32" spans="8:16">
+        <v>99625.36</v>
+      </c>
+      <c r="F10" s="1">
+        <v>99625.36</v>
+      </c>
+      <c r="G10" s="1">
+        <v>374.63639999999998</v>
+      </c>
+      <c r="H10" s="5">
+        <v>8.7401040000000005E-6</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1.763995E-5</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1.001366E-7</v>
+      </c>
+      <c r="K10" s="3">
+        <v>2.648019E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16">
+      <c r="D11" s="1">
+        <v>2000000</v>
+      </c>
+      <c r="E11" s="1">
+        <v>99253.52</v>
+      </c>
+      <c r="F11" s="1">
+        <v>99253.52</v>
+      </c>
+      <c r="G11" s="1">
+        <v>746.47680000000003</v>
+      </c>
+      <c r="H11" s="5">
+        <v>8.707482E-6</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1.7574109999999999E-5</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1.995258E-7</v>
+      </c>
+      <c r="K11" s="3">
+        <v>2.6481120000000001E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16">
+      <c r="D12" s="1">
+        <v>3000000</v>
+      </c>
+      <c r="E12" s="1">
+        <v>98884.45</v>
+      </c>
+      <c r="F12" s="1">
+        <v>98884.45</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1115.5519999999999</v>
+      </c>
+      <c r="H12" s="5">
+        <v>8.6751040000000003E-6</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1.7508760000000001E-5</v>
+      </c>
+      <c r="J12" s="1">
+        <v>2.9817599999999998E-7</v>
+      </c>
+      <c r="K12" s="3">
+        <v>2.6482040000000001E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16">
+      <c r="D13" s="1">
+        <v>4000000</v>
+      </c>
+      <c r="E13" s="1">
+        <v>98518.11</v>
+      </c>
+      <c r="F13" s="1">
+        <v>98518.11</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1481.894</v>
+      </c>
+      <c r="H13" s="5">
+        <v>8.6429649999999993E-6</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1.7443900000000001E-5</v>
+      </c>
+      <c r="J13" s="1">
+        <v>3.960953E-7</v>
+      </c>
+      <c r="K13" s="3">
+        <v>2.6482960000000001E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="3:16">
+      <c r="D14" s="1">
+        <v>5000000</v>
+      </c>
+      <c r="E14" s="1">
+        <v>98154.47</v>
+      </c>
+      <c r="F14" s="1">
+        <v>98154.47</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1845.5309999999999</v>
+      </c>
+      <c r="H14" s="1">
+        <v>8.6110630000000001E-6</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1.7379509999999999E-5</v>
+      </c>
+      <c r="J14" s="1">
+        <v>4.9329199999999999E-7</v>
+      </c>
+      <c r="K14" s="3">
+        <v>2.648386E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="3:16">
+      <c r="D15" s="1">
+        <v>6000000</v>
+      </c>
+      <c r="E15" s="1">
+        <v>97793.51</v>
+      </c>
+      <c r="F15" s="1">
+        <v>97793.51</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2206.4940000000001</v>
+      </c>
+      <c r="H15" s="1">
+        <v>8.5793949999999992E-6</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1.7315600000000001E-5</v>
+      </c>
+      <c r="J15" s="1">
+        <v>5.8977390000000003E-7</v>
+      </c>
+      <c r="K15" s="3">
+        <v>2.6484769999999999E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="3:16">
+      <c r="D16" s="1">
+        <v>7000000</v>
+      </c>
+      <c r="E16" s="1">
+        <v>97435.19</v>
+      </c>
+      <c r="F16" s="1">
+        <v>97435.19</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2564.8130000000001</v>
+      </c>
+      <c r="H16" s="1">
+        <v>8.5479600000000007E-6</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1.725215E-5</v>
+      </c>
+      <c r="J16" s="1">
+        <v>6.8554889999999997E-7</v>
+      </c>
+      <c r="K16" s="3">
+        <v>2.648566E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11">
+      <c r="D17" s="1">
+        <v>8000000</v>
+      </c>
+      <c r="E17" s="1">
+        <v>97079.48</v>
+      </c>
+      <c r="F17" s="1">
+        <v>97079.48</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2920.5160000000001</v>
+      </c>
+      <c r="H17" s="1">
+        <v>8.5167549999999997E-6</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1.7189169999999999E-5</v>
+      </c>
+      <c r="J17" s="1">
+        <v>7.8062479999999995E-7</v>
+      </c>
+      <c r="K17" s="3">
+        <v>2.6486550000000001E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11">
+      <c r="D18" s="1">
+        <v>9000000</v>
+      </c>
+      <c r="E18" s="1">
+        <v>96726.37</v>
+      </c>
+      <c r="F18" s="1">
+        <v>96726.37</v>
+      </c>
+      <c r="G18" s="1">
+        <v>3273.6320000000001</v>
+      </c>
+      <c r="H18" s="2">
+        <v>8.4857760000000003E-6</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1.712665E-5</v>
+      </c>
+      <c r="J18" s="1">
+        <v>8.7500909999999996E-7</v>
+      </c>
+      <c r="K18" s="3">
+        <v>2.6487429999999999E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11">
+      <c r="D19" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="E19" s="1">
+        <v>96375.81</v>
+      </c>
+      <c r="F19" s="1">
+        <v>96375.81</v>
+      </c>
+      <c r="G19" s="1">
+        <v>3624.1889999999999</v>
+      </c>
+      <c r="H19" s="1">
+        <v>8.4550219999999997E-6</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1.7064570000000001E-5</v>
+      </c>
+      <c r="J19" s="1">
+        <v>9.6870939999999994E-7</v>
+      </c>
+      <c r="K19" s="3">
+        <v>2.6488309999999999E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11">
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="3:11">
+      <c r="H22" s="1">
+        <f>E10*4/3*PI()*$E$2^3</f>
+        <v>8.7401006309680879E-6</v>
+      </c>
+      <c r="I22" s="1">
+        <f>F10*4/3*PI()*$F$2^3</f>
+        <v>1.7639950222267175E-5</v>
+      </c>
+      <c r="J22" s="1">
+        <f>G10*4/3*PI()*$G$2^3</f>
+        <v>1.0013655030121573E-7</v>
+      </c>
+      <c r="K22" s="4">
+        <f t="shared" ref="K22:K30" si="0">SUM(H22:J22)</f>
+        <v>2.648018740353648E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11">
+      <c r="H23" s="1">
+        <f t="shared" ref="H23:H31" si="1">E11*4/3*PI()*$E$2^3</f>
+        <v>8.707479227957659E-6</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" ref="I23:I31" si="2">F11*4/3*PI()*$F$2^3</f>
+        <v>1.7574111171942564E-5</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" ref="J23:J31" si="3">G11*4/3*PI()*$G$2^3</f>
+        <v>1.9952575785986243E-7</v>
+      </c>
+      <c r="K23" s="4">
+        <f t="shared" si="0"/>
+        <v>2.6481116157760083E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11">
+      <c r="H24" s="1">
+        <f t="shared" si="1"/>
+        <v>8.6751008361518834E-6</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="2"/>
+        <v>1.7508762585713793E-5</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="3"/>
+        <v>2.9817585520686677E-7</v>
+      </c>
+      <c r="K24" s="4">
+        <f t="shared" si="0"/>
+        <v>2.6482039277072546E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11">
+      <c r="H25" s="1">
+        <f t="shared" si="1"/>
+        <v>8.642961946363693E-6</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="2"/>
+        <v>1.7443897381066851E-5</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="3"/>
+        <v>3.9609539562111373E-7</v>
+      </c>
+      <c r="K25" s="4">
+        <f t="shared" si="0"/>
+        <v>2.6482954723051659E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11">
+      <c r="H26" s="1">
+        <f t="shared" si="1"/>
+        <v>8.6110599267027817E-6</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="2"/>
+        <v>1.7379510246116217E-5</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="3"/>
+        <v>4.932919166796206E-7</v>
+      </c>
+      <c r="K26" s="4">
+        <f t="shared" si="0"/>
+        <v>2.6483862089498621E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11">
+      <c r="H27" s="1">
+        <f t="shared" si="1"/>
+        <v>8.5793930225756189E-6</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="2"/>
+        <v>1.7315597639604891E-5</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="3"/>
+        <v>5.8977370437130712E-7</v>
+      </c>
+      <c r="K27" s="4">
+        <f t="shared" si="0"/>
+        <v>2.6484764366551816E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11">
+      <c r="H28" s="1">
+        <f t="shared" si="1"/>
+        <v>8.5479577247951281E-6</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="2"/>
+        <v>1.7252152479018842E-5</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" si="3"/>
+        <v>6.855487773951278E-7</v>
+      </c>
+      <c r="K28" s="4">
+        <f t="shared" si="0"/>
+        <v>2.6485658981209097E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11">
+      <c r="H29" s="1">
+        <f t="shared" si="1"/>
+        <v>8.5167514014710102E-6</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="2"/>
+        <v>1.7189169452472562E-5</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="3"/>
+        <v>7.8062461987010722E-7</v>
+      </c>
+      <c r="K29" s="4">
+        <f t="shared" si="0"/>
+        <v>2.6486545473813681E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11">
+      <c r="H30" s="1">
+        <f t="shared" si="1"/>
+        <v>8.4857731753064963E-6</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="2"/>
+        <v>1.7126646789337548E-5</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="3"/>
+        <v>8.7500898320523446E-7</v>
+      </c>
+      <c r="K30" s="4">
+        <f t="shared" si="0"/>
+        <v>2.6487428947849278E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11">
+      <c r="H31" s="1">
+        <f t="shared" si="1"/>
+        <v>8.455018659817748E-6</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="2"/>
+        <v>1.7064575636471267E-5</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" si="3"/>
+        <v>9.6870935151953409E-7</v>
+      </c>
+      <c r="K31" s="4">
+        <f>SUM(H31:J31)</f>
+        <v>2.6488303647808552E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11">
       <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="8:8">
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="8:10">
       <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>